<commit_message>
updated excel file and and app.py
</commit_message>
<xml_diff>
--- a/Project01_ProcessingExcelSpreadsheet/transactions.xlsx
+++ b/Project01_ProcessingExcelSpreadsheet/transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonam/Documents/Python/Project01_ProcessingExcelSpreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10A466CC-F87B-EE42-B50F-F287F292E5EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78573F60-F490-6845-8B1F-3D3F00B6A8E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="0" windowWidth="10000" windowHeight="17440" xr2:uid="{CD974221-F5D7-7A47-B188-ED8F8FE3485A}"/>
+    <workbookView xWindow="1280" yWindow="0" windowWidth="15580" windowHeight="17440" xr2:uid="{CD974221-F5D7-7A47-B188-ED8F8FE3485A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8763FA3E-C63D-EF44-9A6E-F4DAB4AB338A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -402,7 +402,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -423,11 +423,8 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>5.3550000000000004</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -437,11 +434,8 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>6.2549999999999999</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -450,9 +444,6 @@
       </c>
       <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="D4">
-        <v>7.1550000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>